<commit_message>
ERD, UML en database voorbeeld
</commit_message>
<xml_diff>
--- a/Ontwerpen/Ontwerpen_OptioneelNietLeegFormaat_Waarderen_32025INF1_Maarten_Kampmeijer.xlsx
+++ b/Ontwerpen/Ontwerpen_OptioneelNietLeegFormaat_Waarderen_32025INF1_Maarten_Kampmeijer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Avans\Ontwerpen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD78516D-61B5-4E10-9290-23BC5080A205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612B973-D5AB-4D4F-B5BC-152441EE8344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="4" activeTab="6" xr2:uid="{380EDD82-D72C-4873-8622-D29EF5813698}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{380EDD82-D72C-4873-8622-D29EF5813698}"/>
   </bookViews>
   <sheets>
     <sheet name="Verwoorden etc." sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="195">
   <si>
     <t>i1</t>
   </si>
@@ -4427,296 +4427,6 @@
     <t xml:space="preserve">2. Binnen de verzamelingen van alle combinaties van soort en variant </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color theme="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>starttijd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>starttijd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">en </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color theme="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>locatie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>locatienaam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. De taart van de </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color theme="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>soort</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>soortnaam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&gt; start op </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&gt; en </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>startijd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>starttijd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&gt; uur op </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color theme="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>locatie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>locatienaam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3. Binnen de verzamelingen van alle combinaties van datum, starttijd en locatie identificeert de combinatie </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="8"/>
-        <color theme="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;,</t>
-    </r>
-  </si>
-  <si>
     <t>Tekst</t>
   </si>
   <si>
@@ -4724,6 +4434,205 @@
   </si>
   <si>
     <t>Getal</t>
+  </si>
+  <si>
+    <t>buurtbewonernaam</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color theme="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Buurtbewoner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>buurtbewonernaam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; schrijft zich in voor het taart bakken van de </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color theme="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>soort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>soortnaam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; voor de </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color theme="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>datum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>datum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; en </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color theme="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>starttijd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>starttijd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; op </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="8"/>
+        <color theme="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>locatie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>locatienaam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>TaartMetSoortVoorMaximaalAantalPersonen</t>
+  </si>
+  <si>
+    <t>nl</t>
   </si>
 </sst>
 </file>
@@ -5499,13 +5408,13 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5514,10 +5423,10 @@
     <xf numFmtId="20" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -17445,6 +17354,7 @@
     <mergeCell ref="BZ61:CB61"/>
     <mergeCell ref="CC61:CE61"/>
     <mergeCell ref="CF61:CH61"/>
+    <mergeCell ref="CC60:CE60"/>
     <mergeCell ref="BZ9:CB9"/>
     <mergeCell ref="CS9:CU9"/>
     <mergeCell ref="DK9:DM9"/>
@@ -17460,6 +17370,7 @@
     <mergeCell ref="CS17:CU17"/>
     <mergeCell ref="BW48:BY48"/>
     <mergeCell ref="BZ48:CH48"/>
+    <mergeCell ref="CS18:CU18"/>
     <mergeCell ref="BG63:BI63"/>
     <mergeCell ref="BJ63:BL63"/>
     <mergeCell ref="BM63:BO63"/>
@@ -17490,7 +17401,6 @@
     <mergeCell ref="U61:W61"/>
     <mergeCell ref="X61:Z61"/>
     <mergeCell ref="AN61:AP61"/>
-    <mergeCell ref="CS18:CU18"/>
     <mergeCell ref="BJ59:BL59"/>
     <mergeCell ref="BM59:BO59"/>
     <mergeCell ref="B60:D60"/>
@@ -17505,7 +17415,6 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="BW60:BY60"/>
     <mergeCell ref="BZ60:CB60"/>
-    <mergeCell ref="CC60:CE60"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="U18:W18"/>
     <mergeCell ref="AN18:AP18"/>
@@ -17536,8 +17445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34A6EBF-9FD1-4671-A818-3FC5ADD9D83D}">
   <dimension ref="A1:XDN123"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ34" workbookViewId="0">
-      <selection activeCell="CO40" sqref="CO40"/>
+    <sheetView topLeftCell="BS36" workbookViewId="0">
+      <selection activeCell="BV39" activeCellId="3" sqref="BV59:CK64 BX58:CK58 BV58 BV39:CK57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22345,36 +22254,39 @@
     <mergeCell ref="U9:W9"/>
     <mergeCell ref="AN9:AP9"/>
     <mergeCell ref="DK17:DM17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="AN18:AP18"/>
-    <mergeCell ref="BG18:BI18"/>
-    <mergeCell ref="BZ18:CB18"/>
     <mergeCell ref="CS18:CU18"/>
     <mergeCell ref="DK18:DM18"/>
     <mergeCell ref="DK19:DM19"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="U47:Z47"/>
     <mergeCell ref="BG47:BO47"/>
+    <mergeCell ref="BZ19:CB19"/>
+    <mergeCell ref="CS19:CU19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="AN18:AP18"/>
+    <mergeCell ref="BG18:BI18"/>
+    <mergeCell ref="BZ18:CB18"/>
+    <mergeCell ref="AQ48:AS48"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="AN19:AP19"/>
+    <mergeCell ref="BG19:BI19"/>
+    <mergeCell ref="BG48:BI48"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="U48:W48"/>
     <mergeCell ref="X48:Z48"/>
     <mergeCell ref="AN48:AP48"/>
-    <mergeCell ref="AQ48:AS48"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="AN19:AP19"/>
-    <mergeCell ref="BG19:BI19"/>
-    <mergeCell ref="BZ19:CB19"/>
-    <mergeCell ref="CS19:CU19"/>
-    <mergeCell ref="BG48:BI48"/>
     <mergeCell ref="BJ48:BL48"/>
     <mergeCell ref="BM48:BO48"/>
     <mergeCell ref="BW48:BY48"/>
     <mergeCell ref="BZ48:CH48"/>
     <mergeCell ref="CC59:CE59"/>
     <mergeCell ref="CF59:CH59"/>
+    <mergeCell ref="BM59:BO59"/>
+    <mergeCell ref="BW59:BY59"/>
+    <mergeCell ref="BZ59:CB59"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="U60:W60"/>
@@ -22385,9 +22297,6 @@
     <mergeCell ref="BJ60:BL60"/>
     <mergeCell ref="BG59:BI59"/>
     <mergeCell ref="BJ59:BL59"/>
-    <mergeCell ref="BM59:BO59"/>
-    <mergeCell ref="BW59:BY59"/>
-    <mergeCell ref="BZ59:CB59"/>
     <mergeCell ref="B61:D61"/>
     <mergeCell ref="E61:G61"/>
     <mergeCell ref="U61:W61"/>
@@ -22440,8 +22349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9713A7D2-4E2E-452A-913E-FB97AEFAE3CD}">
   <dimension ref="A1:XDN123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="BZ39" workbookViewId="0">
+      <selection activeCell="BW40" sqref="BW40:CM65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24042,32 +23951,34 @@
       </c>
       <c r="BU40" s="3"/>
       <c r="BV40" s="2"/>
-      <c r="BW40" s="3">
+      <c r="BW40" s="2"/>
+      <c r="BX40" s="3">
         <v>6</v>
       </c>
-      <c r="BX40" s="3"/>
-      <c r="BY40" s="1"/>
-      <c r="BZ40" s="2"/>
-      <c r="CA40" s="3">
+      <c r="BY40" s="3"/>
+      <c r="BZ40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CA40" s="2"/>
+      <c r="CB40" s="3">
         <v>1</v>
       </c>
-      <c r="CB40" s="2"/>
       <c r="CC40" s="2"/>
-      <c r="CD40" s="3">
+      <c r="CD40" s="2"/>
+      <c r="CE40" s="3">
         <v>2</v>
       </c>
-      <c r="CE40" s="2"/>
       <c r="CF40" s="2"/>
-      <c r="CG40" s="3">
+      <c r="CG40" s="2"/>
+      <c r="CH40" s="3">
         <v>3</v>
       </c>
-      <c r="CH40" s="2"/>
       <c r="CI40" s="2"/>
-      <c r="CJ40" s="3">
+      <c r="CJ40" s="2"/>
+      <c r="CK40" s="3">
         <v>4</v>
       </c>
-      <c r="CK40" s="3"/>
-      <c r="CL40" s="2"/>
+      <c r="CL40" s="3"/>
       <c r="CM40" s="3">
         <v>5</v>
       </c>
@@ -24078,7 +23989,7 @@
       </c>
       <c r="CQ40" s="3"/>
       <c r="CR40" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="CS40" s="2"/>
       <c r="CT40" s="3">
@@ -24219,21 +24130,21 @@
       <c r="BU41" s="3"/>
       <c r="BV41" s="2"/>
       <c r="BW41" s="2"/>
-      <c r="BX41" s="3"/>
-      <c r="BY41" s="4"/>
-      <c r="BZ41" s="2"/>
-      <c r="CA41" s="3"/>
-      <c r="CB41" s="2"/>
+      <c r="BX41" s="2"/>
+      <c r="BY41" s="3"/>
+      <c r="BZ41" s="4"/>
+      <c r="CA41" s="2"/>
+      <c r="CB41" s="3"/>
       <c r="CC41" s="2"/>
-      <c r="CD41" s="3"/>
-      <c r="CE41" s="2"/>
+      <c r="CD41" s="2"/>
+      <c r="CE41" s="3"/>
       <c r="CF41" s="2"/>
-      <c r="CG41" s="3"/>
-      <c r="CH41" s="2"/>
+      <c r="CG41" s="2"/>
+      <c r="CH41" s="3"/>
       <c r="CI41" s="2"/>
       <c r="CJ41" s="2"/>
-      <c r="CK41" s="3"/>
-      <c r="CL41" s="2"/>
+      <c r="CK41" s="2"/>
+      <c r="CL41" s="3"/>
       <c r="CM41" s="2"/>
       <c r="CN41" s="3"/>
       <c r="CO41" s="2"/>
@@ -24359,14 +24270,16 @@
       <c r="BU42" s="8"/>
       <c r="BV42" s="2"/>
       <c r="BW42" s="2"/>
-      <c r="BX42" s="3"/>
-      <c r="BY42" s="5"/>
-      <c r="BZ42" s="6"/>
-      <c r="CA42" s="7"/>
-      <c r="CB42" s="38"/>
+      <c r="BX42" s="2"/>
+      <c r="BY42" s="3"/>
+      <c r="BZ42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="CA42" s="6"/>
+      <c r="CB42" s="7"/>
       <c r="CC42" s="38"/>
-      <c r="CD42" s="39"/>
-      <c r="CE42" s="2"/>
+      <c r="CD42" s="38"/>
+      <c r="CE42" s="39"/>
       <c r="CF42" s="2"/>
       <c r="CG42" s="2"/>
       <c r="CH42" s="2"/>
@@ -24472,27 +24385,29 @@
       </c>
       <c r="AO47" s="87"/>
       <c r="AP47" s="88"/>
-      <c r="BG47" s="90"/>
-      <c r="BH47" s="90"/>
-      <c r="BI47" s="90"/>
-      <c r="BJ47" s="90"/>
-      <c r="BK47" s="90"/>
-      <c r="BL47" s="90"/>
-      <c r="BM47" s="90"/>
-      <c r="BN47" s="90"/>
-      <c r="BO47" s="90"/>
-      <c r="BW47"/>
+      <c r="BG47" s="92"/>
+      <c r="BH47" s="92"/>
+      <c r="BI47" s="92"/>
+      <c r="BJ47" s="92"/>
+      <c r="BK47" s="92"/>
+      <c r="BL47" s="92"/>
+      <c r="BM47" s="92"/>
+      <c r="BN47" s="92"/>
+      <c r="BO47" s="92"/>
       <c r="BX47"/>
       <c r="BY47"/>
-      <c r="BZ47" s="100"/>
-      <c r="CA47" s="100"/>
-      <c r="CB47" s="100"/>
-      <c r="CC47" s="100"/>
-      <c r="CD47" s="100"/>
-      <c r="CE47" s="100"/>
-      <c r="CF47" s="100"/>
-      <c r="CG47" s="100"/>
-      <c r="CH47" s="100"/>
+      <c r="BZ47"/>
+      <c r="CA47" s="86" t="s">
+        <v>166</v>
+      </c>
+      <c r="CB47" s="87"/>
+      <c r="CC47" s="87"/>
+      <c r="CD47" s="87"/>
+      <c r="CE47" s="87"/>
+      <c r="CF47" s="87"/>
+      <c r="CG47" s="87"/>
+      <c r="CH47" s="87"/>
+      <c r="CI47" s="88"/>
       <c r="CP47"/>
       <c r="CT47"/>
       <c r="CU47"/>
@@ -24544,27 +24459,31 @@
       </c>
       <c r="AR48" s="81"/>
       <c r="AS48" s="82"/>
-      <c r="BG48" s="90"/>
-      <c r="BH48" s="90"/>
-      <c r="BI48" s="90"/>
-      <c r="BJ48" s="90"/>
-      <c r="BK48" s="90"/>
-      <c r="BL48" s="90"/>
-      <c r="BM48" s="90"/>
-      <c r="BN48" s="90"/>
-      <c r="BO48" s="90"/>
-      <c r="BW48" s="90"/>
-      <c r="BX48" s="90"/>
-      <c r="BY48" s="90"/>
-      <c r="BZ48" s="90"/>
-      <c r="CA48" s="90"/>
-      <c r="CB48" s="90"/>
-      <c r="CC48" s="90"/>
-      <c r="CD48" s="90"/>
-      <c r="CE48" s="90"/>
-      <c r="CF48" s="90"/>
-      <c r="CG48" s="90"/>
-      <c r="CH48" s="90"/>
+      <c r="BG48" s="92"/>
+      <c r="BH48" s="92"/>
+      <c r="BI48" s="92"/>
+      <c r="BJ48" s="92"/>
+      <c r="BK48" s="92"/>
+      <c r="BL48" s="92"/>
+      <c r="BM48" s="92"/>
+      <c r="BN48" s="92"/>
+      <c r="BO48" s="92"/>
+      <c r="BX48" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="BY48" s="81"/>
+      <c r="BZ48" s="82"/>
+      <c r="CA48" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="CB48" s="81"/>
+      <c r="CC48" s="81"/>
+      <c r="CD48" s="81"/>
+      <c r="CE48" s="81"/>
+      <c r="CF48" s="81"/>
+      <c r="CG48" s="81"/>
+      <c r="CH48" s="81"/>
+      <c r="CI48" s="82"/>
       <c r="CP48"/>
       <c r="CQ48" s="80" t="s">
         <v>170</v>
@@ -24622,6 +24541,17 @@
         <v>128</v>
       </c>
       <c r="AP49" s="37"/>
+      <c r="CA49" s="35"/>
+      <c r="CB49" s="36"/>
+      <c r="CC49" s="36"/>
+      <c r="CD49" s="36"/>
+      <c r="CE49" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="CF49" s="36"/>
+      <c r="CG49" s="36"/>
+      <c r="CH49" s="36"/>
+      <c r="CI49" s="37"/>
       <c r="CP49"/>
       <c r="CT49"/>
       <c r="CU49"/>
@@ -24695,18 +24625,21 @@
       <c r="BN50" s="2"/>
       <c r="BO50" s="2"/>
       <c r="BV50" s="11"/>
-      <c r="BW50" s="2"/>
-      <c r="BX50" s="2"/>
-      <c r="BY50" s="2"/>
-      <c r="BZ50" s="2"/>
-      <c r="CA50" s="2"/>
-      <c r="CB50" s="2"/>
-      <c r="CC50" s="2"/>
-      <c r="CD50" s="2"/>
-      <c r="CE50" s="2"/>
-      <c r="CF50" s="2"/>
-      <c r="CG50" s="2"/>
-      <c r="CH50" s="2"/>
+      <c r="BW50" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="BX50" s="12"/>
+      <c r="BY50" s="13"/>
+      <c r="BZ50" s="14"/>
+      <c r="CA50" s="12"/>
+      <c r="CB50" s="13"/>
+      <c r="CC50" s="22"/>
+      <c r="CD50" s="12"/>
+      <c r="CE50" s="13"/>
+      <c r="CF50" s="22"/>
+      <c r="CG50" s="12"/>
+      <c r="CH50" s="13"/>
+      <c r="CI50" s="22"/>
       <c r="CP50" s="11" t="s">
         <v>167</v>
       </c>
@@ -24782,17 +24715,26 @@
       <c r="BO51" s="2"/>
       <c r="BV51" s="2"/>
       <c r="BW51" s="2"/>
-      <c r="BX51" s="16"/>
-      <c r="BY51" s="2"/>
-      <c r="BZ51" s="2"/>
-      <c r="CA51" s="16"/>
-      <c r="CB51" s="2"/>
-      <c r="CC51" s="2"/>
-      <c r="CD51" s="16"/>
-      <c r="CE51" s="2"/>
-      <c r="CF51" s="2"/>
-      <c r="CG51" s="16"/>
-      <c r="CH51" s="2"/>
+      <c r="BX51" s="15"/>
+      <c r="BY51" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="BZ51" s="17"/>
+      <c r="CA51" s="15"/>
+      <c r="CB51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC51" s="23"/>
+      <c r="CD51" s="15"/>
+      <c r="CE51" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="CF51" s="23"/>
+      <c r="CG51" s="15"/>
+      <c r="CH51" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="CI51" s="23"/>
       <c r="CP51" s="2"/>
       <c r="CQ51" s="15"/>
       <c r="CR51" s="16" t="s">
@@ -24864,17 +24806,18 @@
       <c r="BO52" s="2"/>
       <c r="BV52" s="2"/>
       <c r="BW52" s="2"/>
-      <c r="BX52" s="2"/>
-      <c r="BY52" s="2"/>
-      <c r="BZ52" s="2"/>
-      <c r="CA52" s="2"/>
-      <c r="CB52" s="2"/>
-      <c r="CC52" s="2"/>
-      <c r="CD52" s="2"/>
-      <c r="CE52" s="2"/>
-      <c r="CF52" s="2"/>
-      <c r="CG52" s="2"/>
-      <c r="CH52" s="2"/>
+      <c r="BX52" s="18"/>
+      <c r="BY52" s="19"/>
+      <c r="BZ52" s="20"/>
+      <c r="CA52" s="18"/>
+      <c r="CB52" s="19"/>
+      <c r="CC52" s="24"/>
+      <c r="CD52" s="18"/>
+      <c r="CE52" s="19"/>
+      <c r="CF52" s="24"/>
+      <c r="CG52" s="18"/>
+      <c r="CH52" s="19"/>
+      <c r="CI52" s="24"/>
       <c r="CP52" s="2"/>
       <c r="CQ52" s="18"/>
       <c r="CR52" s="19"/>
@@ -24947,6 +24890,7 @@
       <c r="CF53" s="2"/>
       <c r="CG53" s="2"/>
       <c r="CH53" s="2"/>
+      <c r="CI53" s="2"/>
       <c r="CP53" s="2"/>
       <c r="CQ53" s="2"/>
       <c r="CR53" s="2"/>
@@ -24991,10 +24935,12 @@
       <c r="BG54" s="21"/>
       <c r="BJ54" s="21"/>
       <c r="BM54" s="21"/>
-      <c r="BW54" s="26"/>
-      <c r="BZ54" s="25"/>
-      <c r="CC54" s="25"/>
-      <c r="CF54" s="25"/>
+      <c r="BX54" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="CA54" s="25"/>
+      <c r="CD54" s="25"/>
+      <c r="CG54" s="25"/>
       <c r="CQ54" s="26" t="s">
         <v>180</v>
       </c>
@@ -25033,13 +24979,13 @@
       <c r="BG55" s="21"/>
       <c r="BJ55" s="21"/>
       <c r="BM55" s="21"/>
-      <c r="BW55" s="26"/>
-      <c r="BZ55" s="25"/>
-      <c r="CC55" s="25"/>
-      <c r="CF55" s="25"/>
-      <c r="CQ55" s="26" t="s">
-        <v>189</v>
-      </c>
+      <c r="BX55" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="CA55" s="25"/>
+      <c r="CD55" s="25"/>
+      <c r="CG55" s="25"/>
+      <c r="CQ55" s="26"/>
       <c r="CT55" s="25"/>
       <c r="CW55" s="25"/>
       <c r="CZ55" s="25"/>
@@ -25076,19 +25022,16 @@
       <c r="BG56" s="21"/>
       <c r="BJ56" s="21"/>
       <c r="BM56" s="21"/>
-      <c r="BW56" s="26"/>
-      <c r="BZ56" s="25"/>
-      <c r="CC56" s="25"/>
-      <c r="CF56" s="25"/>
-      <c r="CQ56" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="CT56" s="25"/>
+      <c r="BX56" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="CA56" s="25"/>
+      <c r="CD56" s="25"/>
+      <c r="CG56" s="25"/>
+      <c r="CQ56" s="26"/>
       <c r="CW56" s="25"/>
       <c r="CZ56" s="25"/>
-      <c r="DD56" s="26" t="s">
-        <v>188</v>
-      </c>
+      <c r="DD56" s="26"/>
       <c r="DG56" s="25"/>
       <c r="EA56"/>
       <c r="EB56"/>
@@ -25121,13 +25064,11 @@
       <c r="BG57" s="25"/>
       <c r="BJ57" s="25"/>
       <c r="BM57" s="25"/>
-      <c r="BW57" s="26"/>
-      <c r="BZ57" s="25"/>
-      <c r="CC57" s="25"/>
-      <c r="CF57" s="25"/>
-      <c r="CQ57" s="26" t="s">
-        <v>145</v>
-      </c>
+      <c r="BX57" s="26"/>
+      <c r="CA57" s="25"/>
+      <c r="CD57" s="25"/>
+      <c r="CG57" s="25"/>
+      <c r="CQ57" s="26"/>
       <c r="CT57" s="25"/>
       <c r="CW57" s="25"/>
       <c r="CZ57" s="25"/>
@@ -25156,6 +25097,9 @@
       <c r="AQ58" s="25"/>
       <c r="BF58" s="11"/>
       <c r="BV58" s="11"/>
+      <c r="BW58" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="EA58"/>
       <c r="EB58"/>
       <c r="EC58"/>
@@ -25186,28 +25130,42 @@
         <v>9</v>
       </c>
       <c r="BF59" s="11"/>
-      <c r="BG59" s="95"/>
-      <c r="BH59" s="90"/>
-      <c r="BI59" s="90"/>
+      <c r="BG59" s="96"/>
+      <c r="BH59" s="92"/>
+      <c r="BI59" s="92"/>
       <c r="BJ59" s="93"/>
-      <c r="BK59" s="90"/>
-      <c r="BL59" s="90"/>
-      <c r="BM59" s="90"/>
-      <c r="BN59" s="90"/>
-      <c r="BO59" s="90"/>
+      <c r="BK59" s="92"/>
+      <c r="BL59" s="92"/>
+      <c r="BM59" s="92"/>
+      <c r="BN59" s="92"/>
+      <c r="BO59" s="92"/>
       <c r="BV59" s="11"/>
-      <c r="BW59" s="90"/>
-      <c r="BX59" s="90"/>
-      <c r="BY59" s="90"/>
-      <c r="BZ59" s="95"/>
-      <c r="CA59" s="90"/>
-      <c r="CB59" s="90"/>
-      <c r="CC59" s="93"/>
-      <c r="CD59" s="90"/>
-      <c r="CE59" s="90"/>
-      <c r="CF59" s="90"/>
-      <c r="CG59" s="90"/>
-      <c r="CH59" s="90"/>
+      <c r="BW59" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="BX59" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY59" s="71"/>
+      <c r="BZ59" s="71"/>
+      <c r="CA59" s="75">
+        <v>45912</v>
+      </c>
+      <c r="CB59" s="71"/>
+      <c r="CC59" s="72"/>
+      <c r="CD59" s="76">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="CE59" s="71"/>
+      <c r="CF59" s="72"/>
+      <c r="CG59" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH59" s="78"/>
+      <c r="CI59" s="79"/>
+      <c r="CJ59" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="CP59" s="11" t="s">
         <v>9</v>
       </c>
@@ -25273,36 +25231,50 @@
         <v>126</v>
       </c>
       <c r="BF60" s="11"/>
-      <c r="BG60" s="95"/>
-      <c r="BH60" s="90"/>
-      <c r="BI60" s="90"/>
+      <c r="BG60" s="96"/>
+      <c r="BH60" s="92"/>
+      <c r="BI60" s="92"/>
       <c r="BJ60" s="93"/>
-      <c r="BK60" s="90"/>
-      <c r="BL60" s="90"/>
-      <c r="BM60" s="90"/>
-      <c r="BN60" s="90"/>
-      <c r="BO60" s="90"/>
+      <c r="BK60" s="92"/>
+      <c r="BL60" s="92"/>
+      <c r="BM60" s="92"/>
+      <c r="BN60" s="92"/>
+      <c r="BO60" s="92"/>
       <c r="BV60" s="11"/>
-      <c r="BW60" s="90"/>
-      <c r="BX60" s="90"/>
-      <c r="BY60" s="90"/>
-      <c r="BZ60" s="95"/>
-      <c r="CA60" s="90"/>
-      <c r="CB60" s="90"/>
-      <c r="CC60" s="93"/>
-      <c r="CD60" s="90"/>
-      <c r="CE60" s="90"/>
-      <c r="CF60" s="90"/>
-      <c r="CG60" s="90"/>
-      <c r="CH60" s="90"/>
+      <c r="BW60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BX60" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="BY60" s="52"/>
+      <c r="BZ60" s="52"/>
+      <c r="CA60" s="56">
+        <v>45914</v>
+      </c>
+      <c r="CB60" s="52"/>
+      <c r="CC60" s="42"/>
+      <c r="CD60" s="51">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="CE60" s="52"/>
+      <c r="CF60" s="42"/>
+      <c r="CG60" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH60" s="65"/>
+      <c r="CI60" s="74"/>
+      <c r="CJ60" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="CP60" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="CQ60" s="96" t="s">
+      <c r="CQ60" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="CR60" s="96"/>
-      <c r="CS60" s="96"/>
+      <c r="CR60" s="95"/>
+      <c r="CS60" s="95"/>
       <c r="CT60" s="71" t="s">
         <v>22</v>
       </c>
@@ -25388,28 +25360,42 @@
         <v>13</v>
       </c>
       <c r="BF61" s="11"/>
-      <c r="BG61" s="92"/>
-      <c r="BH61" s="90"/>
-      <c r="BI61" s="90"/>
+      <c r="BG61" s="91"/>
+      <c r="BH61" s="92"/>
+      <c r="BI61" s="92"/>
       <c r="BJ61" s="93"/>
-      <c r="BK61" s="90"/>
-      <c r="BL61" s="90"/>
-      <c r="BM61" s="90"/>
-      <c r="BN61" s="90"/>
-      <c r="BO61" s="90"/>
+      <c r="BK61" s="92"/>
+      <c r="BL61" s="92"/>
+      <c r="BM61" s="92"/>
+      <c r="BN61" s="92"/>
+      <c r="BO61" s="92"/>
       <c r="BV61" s="11"/>
-      <c r="BW61" s="90"/>
-      <c r="BX61" s="90"/>
-      <c r="BY61" s="90"/>
-      <c r="BZ61" s="92"/>
-      <c r="CA61" s="90"/>
-      <c r="CB61" s="90"/>
-      <c r="CC61" s="93"/>
-      <c r="CD61" s="90"/>
-      <c r="CE61" s="90"/>
-      <c r="CF61" s="90"/>
-      <c r="CG61" s="90"/>
-      <c r="CH61" s="90"/>
+      <c r="BW61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="BX61" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="BY61" s="52"/>
+      <c r="BZ61" s="52"/>
+      <c r="CA61" s="59">
+        <v>45914</v>
+      </c>
+      <c r="CB61" s="52"/>
+      <c r="CC61" s="42"/>
+      <c r="CD61" s="64">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="CE61" s="65"/>
+      <c r="CF61" s="66"/>
+      <c r="CG61" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH61" s="61"/>
+      <c r="CI61" s="62"/>
+      <c r="CJ61" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="CP61" s="11" t="s">
         <v>12</v>
       </c>
@@ -25503,28 +25489,39 @@
         <v>16</v>
       </c>
       <c r="BF62" s="11"/>
-      <c r="BG62" s="92"/>
-      <c r="BH62" s="90"/>
-      <c r="BI62" s="90"/>
+      <c r="BG62" s="91"/>
+      <c r="BH62" s="92"/>
+      <c r="BI62" s="92"/>
       <c r="BJ62" s="93"/>
-      <c r="BK62" s="90"/>
-      <c r="BL62" s="90"/>
-      <c r="BM62" s="90"/>
-      <c r="BN62" s="90"/>
-      <c r="BO62" s="90"/>
+      <c r="BK62" s="92"/>
+      <c r="BL62" s="92"/>
+      <c r="BM62" s="92"/>
+      <c r="BN62" s="92"/>
+      <c r="BO62" s="92"/>
       <c r="BV62" s="11"/>
-      <c r="BW62" s="90"/>
-      <c r="BX62" s="90"/>
-      <c r="BY62" s="90"/>
-      <c r="BZ62" s="92"/>
-      <c r="CA62" s="90"/>
-      <c r="CB62" s="90"/>
-      <c r="CC62" s="93"/>
-      <c r="CD62" s="90"/>
-      <c r="CE62" s="90"/>
-      <c r="CF62" s="90"/>
-      <c r="CG62" s="90"/>
-      <c r="CH62" s="90"/>
+      <c r="BW62" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX62" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY62" s="52"/>
+      <c r="BZ62" s="52"/>
+      <c r="CA62" s="68">
+        <v>45914</v>
+      </c>
+      <c r="CB62" s="65"/>
+      <c r="CC62" s="66"/>
+      <c r="CD62" s="51">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="CE62" s="52"/>
+      <c r="CF62" s="42"/>
+      <c r="CG62" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH62" s="61"/>
+      <c r="CI62" s="62"/>
       <c r="CP62" s="11" t="s">
         <v>14</v>
       </c>
@@ -25565,28 +25562,39 @@
     </row>
     <row r="63" spans="1:133 16340:16342">
       <c r="BF63" s="11"/>
-      <c r="BG63" s="92"/>
-      <c r="BH63" s="90"/>
-      <c r="BI63" s="90"/>
+      <c r="BG63" s="91"/>
+      <c r="BH63" s="92"/>
+      <c r="BI63" s="92"/>
       <c r="BJ63" s="93"/>
-      <c r="BK63" s="90"/>
-      <c r="BL63" s="90"/>
-      <c r="BM63" s="90"/>
-      <c r="BN63" s="90"/>
-      <c r="BO63" s="90"/>
+      <c r="BK63" s="92"/>
+      <c r="BL63" s="92"/>
+      <c r="BM63" s="92"/>
+      <c r="BN63" s="92"/>
+      <c r="BO63" s="92"/>
       <c r="BV63" s="11"/>
-      <c r="BW63" s="90"/>
-      <c r="BX63" s="90"/>
-      <c r="BY63" s="90"/>
-      <c r="BZ63" s="92"/>
-      <c r="CA63" s="90"/>
-      <c r="CB63" s="90"/>
-      <c r="CC63" s="93"/>
-      <c r="CD63" s="90"/>
-      <c r="CE63" s="90"/>
-      <c r="CF63" s="90"/>
-      <c r="CG63" s="90"/>
-      <c r="CH63" s="90"/>
+      <c r="BW63" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="BX63" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="BY63" s="63"/>
+      <c r="BZ63" s="63"/>
+      <c r="CA63" s="59">
+        <v>45914</v>
+      </c>
+      <c r="CB63" s="52"/>
+      <c r="CC63" s="42"/>
+      <c r="CD63" s="51">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="CE63" s="52"/>
+      <c r="CF63" s="42"/>
+      <c r="CG63" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH63" s="61"/>
+      <c r="CI63" s="62"/>
       <c r="CP63" s="11" t="s">
         <v>130</v>
       </c>
@@ -25600,7 +25608,7 @@
       </c>
       <c r="CU63" s="52"/>
       <c r="CV63" s="52"/>
-      <c r="CW63" s="91">
+      <c r="CW63" s="90">
         <v>45914</v>
       </c>
       <c r="CX63" s="65"/>
@@ -26722,12 +26730,6 @@
     <mergeCell ref="BG18:BI18"/>
     <mergeCell ref="BZ18:CB18"/>
     <mergeCell ref="CS18:CU18"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="U48:W48"/>
-    <mergeCell ref="X48:Z48"/>
-    <mergeCell ref="AN48:AP48"/>
-    <mergeCell ref="AQ48:AS48"/>
     <mergeCell ref="BG46:BO46"/>
     <mergeCell ref="CQ46:CS46"/>
     <mergeCell ref="CW46:DE46"/>
@@ -26735,36 +26737,25 @@
     <mergeCell ref="U47:Z47"/>
     <mergeCell ref="AN47:AP47"/>
     <mergeCell ref="BG47:BO47"/>
-    <mergeCell ref="BZ47:CH47"/>
     <mergeCell ref="CW47:DE47"/>
     <mergeCell ref="CT48:CV48"/>
     <mergeCell ref="CW48:CY48"/>
     <mergeCell ref="CZ48:DB48"/>
     <mergeCell ref="DC48:DE48"/>
-    <mergeCell ref="CW49:DE49"/>
     <mergeCell ref="BG59:BI59"/>
     <mergeCell ref="BJ59:BL59"/>
     <mergeCell ref="BM59:BO59"/>
-    <mergeCell ref="BW59:BY59"/>
-    <mergeCell ref="BZ59:CB59"/>
     <mergeCell ref="BG48:BI48"/>
     <mergeCell ref="BJ48:BL48"/>
     <mergeCell ref="BM48:BO48"/>
-    <mergeCell ref="BW48:BY48"/>
-    <mergeCell ref="BZ48:CH48"/>
     <mergeCell ref="CQ48:CS48"/>
-    <mergeCell ref="CC59:CE59"/>
-    <mergeCell ref="CF59:CH59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="U60:W60"/>
-    <mergeCell ref="X60:Z60"/>
-    <mergeCell ref="AN60:AP60"/>
-    <mergeCell ref="AQ60:AS60"/>
-    <mergeCell ref="BG60:BI60"/>
-    <mergeCell ref="BJ60:BL60"/>
-    <mergeCell ref="CT60:CV60"/>
-    <mergeCell ref="CW60:CY60"/>
+    <mergeCell ref="CA48:CI48"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="U48:W48"/>
+    <mergeCell ref="X48:Z48"/>
+    <mergeCell ref="AN48:AP48"/>
+    <mergeCell ref="AQ48:AS48"/>
     <mergeCell ref="CZ60:DB60"/>
     <mergeCell ref="DC60:DE60"/>
     <mergeCell ref="B61:D61"/>
@@ -26774,10 +26765,6 @@
     <mergeCell ref="AN61:AP61"/>
     <mergeCell ref="AQ61:AS61"/>
     <mergeCell ref="BM60:BO60"/>
-    <mergeCell ref="BW60:BY60"/>
-    <mergeCell ref="BZ60:CB60"/>
-    <mergeCell ref="CC60:CE60"/>
-    <mergeCell ref="CF60:CH60"/>
     <mergeCell ref="CQ60:CS60"/>
     <mergeCell ref="CW61:CY61"/>
     <mergeCell ref="CZ61:DB61"/>
@@ -26785,45 +26772,39 @@
     <mergeCell ref="BG61:BI61"/>
     <mergeCell ref="BJ61:BL61"/>
     <mergeCell ref="BM61:BO61"/>
-    <mergeCell ref="BW61:BY61"/>
-    <mergeCell ref="BZ61:CB61"/>
-    <mergeCell ref="CC61:CE61"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="U60:W60"/>
+    <mergeCell ref="X60:Z60"/>
+    <mergeCell ref="AN60:AP60"/>
+    <mergeCell ref="AQ60:AS60"/>
+    <mergeCell ref="BG60:BI60"/>
+    <mergeCell ref="BJ60:BL60"/>
+    <mergeCell ref="DC62:DE62"/>
+    <mergeCell ref="BG62:BI62"/>
+    <mergeCell ref="BJ62:BL62"/>
+    <mergeCell ref="BM62:BO62"/>
+    <mergeCell ref="BX62:BZ62"/>
+    <mergeCell ref="CA62:CC62"/>
+    <mergeCell ref="CD62:CF62"/>
+    <mergeCell ref="CG62:CI62"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="U62:W62"/>
     <mergeCell ref="X62:Z62"/>
     <mergeCell ref="AN62:AP62"/>
     <mergeCell ref="AQ62:AS62"/>
-    <mergeCell ref="CF61:CH61"/>
-    <mergeCell ref="CQ61:CS61"/>
-    <mergeCell ref="CT61:CV61"/>
-    <mergeCell ref="CF62:CH62"/>
     <mergeCell ref="CQ62:CS62"/>
     <mergeCell ref="CT62:CV62"/>
-    <mergeCell ref="CW62:CY62"/>
-    <mergeCell ref="CZ62:DB62"/>
-    <mergeCell ref="DC62:DE62"/>
-    <mergeCell ref="BG62:BI62"/>
-    <mergeCell ref="BJ62:BL62"/>
-    <mergeCell ref="BM62:BO62"/>
-    <mergeCell ref="BW62:BY62"/>
-    <mergeCell ref="BZ62:CB62"/>
-    <mergeCell ref="CC62:CE62"/>
-    <mergeCell ref="CF63:CH63"/>
-    <mergeCell ref="CQ63:CS63"/>
-    <mergeCell ref="CT63:CV63"/>
-    <mergeCell ref="CW63:CY63"/>
-    <mergeCell ref="CZ63:DB63"/>
-    <mergeCell ref="DC63:DE63"/>
     <mergeCell ref="BG63:BI63"/>
     <mergeCell ref="BJ63:BL63"/>
     <mergeCell ref="BM63:BO63"/>
-    <mergeCell ref="BW63:BY63"/>
-    <mergeCell ref="BZ63:CB63"/>
-    <mergeCell ref="CC63:CE63"/>
-    <mergeCell ref="CQ64:CS64"/>
-    <mergeCell ref="CT64:CV64"/>
-    <mergeCell ref="CW64:CY64"/>
+    <mergeCell ref="BX63:BZ63"/>
+    <mergeCell ref="CA63:CC63"/>
+    <mergeCell ref="CD63:CF63"/>
+    <mergeCell ref="CG63:CI63"/>
+    <mergeCell ref="CW62:CY62"/>
+    <mergeCell ref="CZ62:DB62"/>
     <mergeCell ref="CZ64:DB64"/>
     <mergeCell ref="DC64:DE64"/>
     <mergeCell ref="CQ65:CS65"/>
@@ -26831,6 +26812,33 @@
     <mergeCell ref="CW65:CY65"/>
     <mergeCell ref="CZ65:DB65"/>
     <mergeCell ref="DC65:DE65"/>
+    <mergeCell ref="CQ63:CS63"/>
+    <mergeCell ref="CT63:CV63"/>
+    <mergeCell ref="CW63:CY63"/>
+    <mergeCell ref="CZ63:DB63"/>
+    <mergeCell ref="DC63:DE63"/>
+    <mergeCell ref="CA47:CI47"/>
+    <mergeCell ref="BX48:BZ48"/>
+    <mergeCell ref="BX59:BZ59"/>
+    <mergeCell ref="CA59:CC59"/>
+    <mergeCell ref="CD59:CF59"/>
+    <mergeCell ref="CG59:CI59"/>
+    <mergeCell ref="CQ64:CS64"/>
+    <mergeCell ref="CT64:CV64"/>
+    <mergeCell ref="CW64:CY64"/>
+    <mergeCell ref="CQ61:CS61"/>
+    <mergeCell ref="CT61:CV61"/>
+    <mergeCell ref="BX61:BZ61"/>
+    <mergeCell ref="CA61:CC61"/>
+    <mergeCell ref="CD61:CF61"/>
+    <mergeCell ref="CG61:CI61"/>
+    <mergeCell ref="CW60:CY60"/>
+    <mergeCell ref="CT60:CV60"/>
+    <mergeCell ref="BX60:BZ60"/>
+    <mergeCell ref="CA60:CC60"/>
+    <mergeCell ref="CD60:CF60"/>
+    <mergeCell ref="CG60:CI60"/>
+    <mergeCell ref="CW49:DE49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26840,8 +26848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E5A712-D8E1-4FAD-A449-B8CCD36028EF}">
   <dimension ref="A1:XDN123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="AK57" sqref="AK57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27841,7 +27849,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
@@ -27858,7 +27866,7 @@
         <v>1</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="V11" s="13"/>
       <c r="W11" s="14"/>
@@ -27866,7 +27874,7 @@
         <v>2</v>
       </c>
       <c r="AN11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AO11" s="13"/>
       <c r="AP11" s="14"/>
@@ -27882,7 +27890,7 @@
         <v>4</v>
       </c>
       <c r="BZ11" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="CA11" s="13"/>
       <c r="CB11" s="14"/>
@@ -27890,7 +27898,7 @@
         <v>5</v>
       </c>
       <c r="CS11" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CT11" s="13"/>
       <c r="CU11" s="14"/>
@@ -27898,7 +27906,7 @@
         <v>108</v>
       </c>
       <c r="DK11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DL11" s="13"/>
       <c r="DM11" s="14"/>
@@ -27946,7 +27954,7 @@
       <c r="CU12" s="17"/>
       <c r="DK12" s="15"/>
       <c r="DL12" s="16" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="DM12" s="17"/>
     </row>
@@ -28456,32 +28464,34 @@
       </c>
       <c r="BU40" s="3"/>
       <c r="BV40" s="2"/>
-      <c r="BW40" s="3">
+      <c r="BW40" s="2"/>
+      <c r="BX40" s="3">
         <v>6</v>
       </c>
-      <c r="BX40" s="3"/>
-      <c r="BY40" s="1"/>
-      <c r="BZ40" s="2"/>
-      <c r="CA40" s="3">
+      <c r="BY40" s="3"/>
+      <c r="BZ40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CA40" s="2"/>
+      <c r="CB40" s="3">
         <v>1</v>
       </c>
-      <c r="CB40" s="2"/>
       <c r="CC40" s="2"/>
-      <c r="CD40" s="3">
+      <c r="CD40" s="2"/>
+      <c r="CE40" s="3">
         <v>2</v>
       </c>
-      <c r="CE40" s="2"/>
       <c r="CF40" s="2"/>
-      <c r="CG40" s="3">
+      <c r="CG40" s="2"/>
+      <c r="CH40" s="3">
         <v>3</v>
       </c>
-      <c r="CH40" s="2"/>
       <c r="CI40" s="2"/>
-      <c r="CJ40" s="3">
+      <c r="CJ40" s="2"/>
+      <c r="CK40" s="3">
         <v>4</v>
       </c>
-      <c r="CK40" s="3"/>
-      <c r="CL40" s="2"/>
+      <c r="CL40" s="3"/>
       <c r="CM40" s="3">
         <v>5</v>
       </c>
@@ -28492,7 +28502,7 @@
       </c>
       <c r="CQ40" s="3"/>
       <c r="CR40" s="1" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="CS40" s="2"/>
       <c r="CT40" s="3">
@@ -28633,21 +28643,21 @@
       <c r="BU41" s="3"/>
       <c r="BV41" s="2"/>
       <c r="BW41" s="2"/>
-      <c r="BX41" s="3"/>
-      <c r="BY41" s="4"/>
-      <c r="BZ41" s="2"/>
-      <c r="CA41" s="3"/>
-      <c r="CB41" s="2"/>
+      <c r="BX41" s="2"/>
+      <c r="BY41" s="3"/>
+      <c r="BZ41" s="4"/>
+      <c r="CA41" s="2"/>
+      <c r="CB41" s="3"/>
       <c r="CC41" s="2"/>
-      <c r="CD41" s="3"/>
-      <c r="CE41" s="2"/>
+      <c r="CD41" s="2"/>
+      <c r="CE41" s="3"/>
       <c r="CF41" s="2"/>
-      <c r="CG41" s="3"/>
-      <c r="CH41" s="2"/>
+      <c r="CG41" s="2"/>
+      <c r="CH41" s="3"/>
       <c r="CI41" s="2"/>
       <c r="CJ41" s="2"/>
-      <c r="CK41" s="3"/>
-      <c r="CL41" s="2"/>
+      <c r="CK41" s="2"/>
+      <c r="CL41" s="3"/>
       <c r="CM41" s="2"/>
       <c r="CN41" s="3"/>
       <c r="CO41" s="2"/>
@@ -28735,7 +28745,7 @@
       <c r="AK42" s="3"/>
       <c r="AL42" s="2"/>
       <c r="AM42" s="5" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="AN42" s="6"/>
       <c r="AO42" s="7"/>
@@ -28773,14 +28783,16 @@
       <c r="BU42" s="8"/>
       <c r="BV42" s="2"/>
       <c r="BW42" s="2"/>
-      <c r="BX42" s="3"/>
-      <c r="BY42" s="5"/>
-      <c r="BZ42" s="6"/>
-      <c r="CA42" s="7"/>
-      <c r="CB42" s="38"/>
+      <c r="BX42" s="2"/>
+      <c r="BY42" s="3"/>
+      <c r="BZ42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="CA42" s="6"/>
+      <c r="CB42" s="7"/>
       <c r="CC42" s="38"/>
-      <c r="CD42" s="39"/>
-      <c r="CE42" s="2"/>
+      <c r="CD42" s="38"/>
+      <c r="CE42" s="39"/>
       <c r="CF42" s="2"/>
       <c r="CG42" s="2"/>
       <c r="CH42" s="2"/>
@@ -28886,27 +28898,29 @@
       </c>
       <c r="AO47" s="87"/>
       <c r="AP47" s="88"/>
-      <c r="BG47" s="90"/>
-      <c r="BH47" s="90"/>
-      <c r="BI47" s="90"/>
-      <c r="BJ47" s="90"/>
-      <c r="BK47" s="90"/>
-      <c r="BL47" s="90"/>
-      <c r="BM47" s="90"/>
-      <c r="BN47" s="90"/>
-      <c r="BO47" s="90"/>
-      <c r="BW47"/>
+      <c r="BG47" s="92"/>
+      <c r="BH47" s="92"/>
+      <c r="BI47" s="92"/>
+      <c r="BJ47" s="92"/>
+      <c r="BK47" s="92"/>
+      <c r="BL47" s="92"/>
+      <c r="BM47" s="92"/>
+      <c r="BN47" s="92"/>
+      <c r="BO47" s="92"/>
       <c r="BX47"/>
       <c r="BY47"/>
-      <c r="BZ47" s="100"/>
-      <c r="CA47" s="100"/>
-      <c r="CB47" s="100"/>
-      <c r="CC47" s="100"/>
-      <c r="CD47" s="100"/>
-      <c r="CE47" s="100"/>
-      <c r="CF47" s="100"/>
-      <c r="CG47" s="100"/>
-      <c r="CH47" s="100"/>
+      <c r="BZ47"/>
+      <c r="CA47" s="86" t="s">
+        <v>166</v>
+      </c>
+      <c r="CB47" s="87"/>
+      <c r="CC47" s="87"/>
+      <c r="CD47" s="87"/>
+      <c r="CE47" s="87"/>
+      <c r="CF47" s="87"/>
+      <c r="CG47" s="87"/>
+      <c r="CH47" s="87"/>
+      <c r="CI47" s="88"/>
       <c r="CP47"/>
       <c r="CT47"/>
       <c r="CU47"/>
@@ -28958,27 +28972,31 @@
       </c>
       <c r="AR48" s="81"/>
       <c r="AS48" s="82"/>
-      <c r="BG48" s="90"/>
-      <c r="BH48" s="90"/>
-      <c r="BI48" s="90"/>
-      <c r="BJ48" s="90"/>
-      <c r="BK48" s="90"/>
-      <c r="BL48" s="90"/>
-      <c r="BM48" s="90"/>
-      <c r="BN48" s="90"/>
-      <c r="BO48" s="90"/>
-      <c r="BW48" s="90"/>
-      <c r="BX48" s="90"/>
-      <c r="BY48" s="90"/>
-      <c r="BZ48" s="90"/>
-      <c r="CA48" s="90"/>
-      <c r="CB48" s="90"/>
-      <c r="CC48" s="90"/>
-      <c r="CD48" s="90"/>
-      <c r="CE48" s="90"/>
-      <c r="CF48" s="90"/>
-      <c r="CG48" s="90"/>
-      <c r="CH48" s="90"/>
+      <c r="BG48" s="92"/>
+      <c r="BH48" s="92"/>
+      <c r="BI48" s="92"/>
+      <c r="BJ48" s="92"/>
+      <c r="BK48" s="92"/>
+      <c r="BL48" s="92"/>
+      <c r="BM48" s="92"/>
+      <c r="BN48" s="92"/>
+      <c r="BO48" s="92"/>
+      <c r="BX48" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="BY48" s="81"/>
+      <c r="BZ48" s="82"/>
+      <c r="CA48" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="CB48" s="81"/>
+      <c r="CC48" s="81"/>
+      <c r="CD48" s="81"/>
+      <c r="CE48" s="81"/>
+      <c r="CF48" s="81"/>
+      <c r="CG48" s="81"/>
+      <c r="CH48" s="81"/>
+      <c r="CI48" s="82"/>
       <c r="CP48"/>
       <c r="CQ48" s="80" t="s">
         <v>170</v>
@@ -29036,6 +29054,17 @@
         <v>128</v>
       </c>
       <c r="AP49" s="37"/>
+      <c r="CA49" s="35"/>
+      <c r="CB49" s="36"/>
+      <c r="CC49" s="36"/>
+      <c r="CD49" s="36"/>
+      <c r="CE49" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="CF49" s="36"/>
+      <c r="CG49" s="36"/>
+      <c r="CH49" s="36"/>
+      <c r="CI49" s="37"/>
       <c r="CP49"/>
       <c r="CT49"/>
       <c r="CU49"/>
@@ -29065,12 +29094,12 @@
         <v>17</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="14"/>
       <c r="E50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="22"/>
@@ -29082,12 +29111,12 @@
         <v>18</v>
       </c>
       <c r="U50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="V50" s="13"/>
       <c r="W50" s="14"/>
       <c r="X50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Y50" s="13"/>
       <c r="Z50" s="22"/>
@@ -29100,12 +29129,12 @@
         <v>19</v>
       </c>
       <c r="AN50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AO50" s="13"/>
       <c r="AP50" s="14"/>
       <c r="AQ50" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AR50" s="13"/>
       <c r="AS50" s="22"/>
@@ -29121,28 +29150,39 @@
       <c r="BN50" s="2"/>
       <c r="BO50" s="2"/>
       <c r="BV50" s="11"/>
-      <c r="BW50" s="2"/>
-      <c r="BX50" s="2"/>
-      <c r="BY50" s="2"/>
-      <c r="BZ50" s="2"/>
-      <c r="CA50" s="2"/>
-      <c r="CB50" s="2"/>
-      <c r="CC50" s="2"/>
-      <c r="CD50" s="2"/>
-      <c r="CE50" s="2"/>
-      <c r="CF50" s="2"/>
-      <c r="CG50" s="2"/>
-      <c r="CH50" s="2"/>
+      <c r="BW50" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="BX50" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="BY50" s="13"/>
+      <c r="BZ50" s="14"/>
+      <c r="CA50" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="CB50" s="13"/>
+      <c r="CC50" s="22"/>
+      <c r="CD50" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="CE50" s="13"/>
+      <c r="CF50" s="22"/>
+      <c r="CG50" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="CH50" s="13"/>
+      <c r="CI50" s="22"/>
       <c r="CP50" s="11" t="s">
         <v>20</v>
       </c>
       <c r="CQ50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CR50" s="13"/>
       <c r="CS50" s="14"/>
       <c r="CT50" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="CU50" s="13"/>
       <c r="CV50" s="14"/>
@@ -29152,12 +29192,12 @@
       <c r="CX50" s="13"/>
       <c r="CY50" s="22"/>
       <c r="CZ50" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="DA50" s="13"/>
       <c r="DB50" s="22"/>
       <c r="DC50" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="DD50" s="13"/>
       <c r="DE50" s="22"/>
@@ -29218,21 +29258,30 @@
       <c r="BO51" s="2"/>
       <c r="BV51" s="2"/>
       <c r="BW51" s="2"/>
-      <c r="BX51" s="16"/>
-      <c r="BY51" s="2"/>
-      <c r="BZ51" s="2"/>
-      <c r="CA51" s="16"/>
-      <c r="CB51" s="2"/>
-      <c r="CC51" s="2"/>
-      <c r="CD51" s="16"/>
-      <c r="CE51" s="2"/>
-      <c r="CF51" s="2"/>
-      <c r="CG51" s="16"/>
-      <c r="CH51" s="2"/>
+      <c r="BX51" s="15"/>
+      <c r="BY51" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="BZ51" s="17"/>
+      <c r="CA51" s="15"/>
+      <c r="CB51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC51" s="23"/>
+      <c r="CD51" s="15"/>
+      <c r="CE51" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="CF51" s="23"/>
+      <c r="CG51" s="15"/>
+      <c r="CH51" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="CI51" s="23"/>
       <c r="CP51" s="2"/>
       <c r="CQ51" s="15"/>
       <c r="CR51" s="16" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="CS51" s="17"/>
       <c r="CT51" s="15"/>
@@ -29286,7 +29335,9 @@
       <c r="AP52" s="20"/>
       <c r="AQ52" s="18"/>
       <c r="AR52" s="19"/>
-      <c r="AS52" s="24"/>
+      <c r="AS52" s="24" t="s">
+        <v>194</v>
+      </c>
       <c r="AT52" s="2"/>
       <c r="BF52" s="2"/>
       <c r="BG52" s="2"/>
@@ -29300,24 +29351,31 @@
       <c r="BO52" s="2"/>
       <c r="BV52" s="2"/>
       <c r="BW52" s="2"/>
-      <c r="BX52" s="2"/>
-      <c r="BY52" s="2"/>
-      <c r="BZ52" s="2"/>
-      <c r="CA52" s="2"/>
-      <c r="CB52" s="2"/>
-      <c r="CC52" s="2"/>
-      <c r="CD52" s="2"/>
-      <c r="CE52" s="2"/>
-      <c r="CF52" s="2"/>
-      <c r="CG52" s="2"/>
-      <c r="CH52" s="2"/>
+      <c r="BX52" s="18"/>
+      <c r="BY52" s="19"/>
+      <c r="BZ52" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="CA52" s="18"/>
+      <c r="CB52" s="19"/>
+      <c r="CC52" s="41"/>
+      <c r="CD52" s="18"/>
+      <c r="CE52" s="19"/>
+      <c r="CF52" s="41"/>
+      <c r="CG52" s="18"/>
+      <c r="CH52" s="19"/>
+      <c r="CI52" s="41"/>
       <c r="CP52" s="2"/>
       <c r="CQ52" s="18"/>
       <c r="CR52" s="19"/>
-      <c r="CS52" s="40"/>
+      <c r="CS52" s="40" t="s">
+        <v>194</v>
+      </c>
       <c r="CT52" s="18"/>
       <c r="CU52" s="19"/>
-      <c r="CV52" s="40"/>
+      <c r="CV52" s="40" t="s">
+        <v>194</v>
+      </c>
       <c r="CW52" s="18"/>
       <c r="CX52" s="19"/>
       <c r="CY52" s="41"/>
@@ -29383,6 +29441,7 @@
       <c r="CF53" s="2"/>
       <c r="CG53" s="2"/>
       <c r="CH53" s="2"/>
+      <c r="CI53" s="2"/>
       <c r="CP53" s="2"/>
       <c r="CQ53" s="2"/>
       <c r="CR53" s="2"/>
@@ -29427,12 +29486,14 @@
       <c r="BG54" s="21"/>
       <c r="BJ54" s="21"/>
       <c r="BM54" s="21"/>
-      <c r="BW54" s="26"/>
-      <c r="BZ54" s="25"/>
-      <c r="CC54" s="25"/>
-      <c r="CF54" s="25"/>
+      <c r="BX54" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="CA54" s="25"/>
+      <c r="CD54" s="25"/>
+      <c r="CG54" s="25"/>
       <c r="CQ54" s="26" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="CT54" s="26"/>
       <c r="CW54" s="25"/>
@@ -29469,13 +29530,13 @@
       <c r="BG55" s="21"/>
       <c r="BJ55" s="21"/>
       <c r="BM55" s="21"/>
-      <c r="BW55" s="26"/>
-      <c r="BZ55" s="25"/>
-      <c r="CC55" s="25"/>
-      <c r="CF55" s="25"/>
-      <c r="CQ55" s="26" t="s">
-        <v>189</v>
-      </c>
+      <c r="BX55" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="CA55" s="25"/>
+      <c r="CD55" s="25"/>
+      <c r="CG55" s="25"/>
+      <c r="CQ55" s="26"/>
       <c r="CT55" s="25"/>
       <c r="CW55" s="25"/>
       <c r="CZ55" s="25"/>
@@ -29512,19 +29573,17 @@
       <c r="BG56" s="21"/>
       <c r="BJ56" s="21"/>
       <c r="BM56" s="21"/>
-      <c r="BW56" s="26"/>
-      <c r="BZ56" s="25"/>
-      <c r="CC56" s="25"/>
-      <c r="CF56" s="25"/>
-      <c r="CQ56" s="26" t="s">
-        <v>190</v>
-      </c>
+      <c r="BX56" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="CA56" s="25"/>
+      <c r="CD56" s="25"/>
+      <c r="CG56" s="25"/>
+      <c r="CQ56" s="26"/>
       <c r="CT56" s="25"/>
       <c r="CW56" s="25"/>
       <c r="CZ56" s="25"/>
-      <c r="DD56" s="26" t="s">
-        <v>188</v>
-      </c>
+      <c r="DD56" s="26"/>
       <c r="DG56" s="25"/>
       <c r="EA56"/>
       <c r="EB56"/>
@@ -29557,13 +29616,11 @@
       <c r="BG57" s="25"/>
       <c r="BJ57" s="25"/>
       <c r="BM57" s="25"/>
-      <c r="BW57" s="26"/>
-      <c r="BZ57" s="25"/>
-      <c r="CC57" s="25"/>
-      <c r="CF57" s="25"/>
-      <c r="CQ57" s="26" t="s">
-        <v>145</v>
-      </c>
+      <c r="BX57" s="26"/>
+      <c r="CA57" s="25"/>
+      <c r="CD57" s="25"/>
+      <c r="CG57" s="25"/>
+      <c r="CQ57" s="26"/>
       <c r="CT57" s="25"/>
       <c r="CW57" s="25"/>
       <c r="CZ57" s="25"/>
@@ -29592,6 +29649,9 @@
       <c r="AQ58" s="25"/>
       <c r="BF58" s="11"/>
       <c r="BV58" s="11"/>
+      <c r="BW58" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="EA58"/>
       <c r="EB58"/>
       <c r="EC58"/>
@@ -29622,28 +29682,42 @@
         <v>9</v>
       </c>
       <c r="BF59" s="11"/>
-      <c r="BG59" s="95"/>
-      <c r="BH59" s="90"/>
-      <c r="BI59" s="90"/>
+      <c r="BG59" s="96"/>
+      <c r="BH59" s="92"/>
+      <c r="BI59" s="92"/>
       <c r="BJ59" s="93"/>
-      <c r="BK59" s="90"/>
-      <c r="BL59" s="90"/>
-      <c r="BM59" s="90"/>
-      <c r="BN59" s="90"/>
-      <c r="BO59" s="90"/>
+      <c r="BK59" s="92"/>
+      <c r="BL59" s="92"/>
+      <c r="BM59" s="92"/>
+      <c r="BN59" s="92"/>
+      <c r="BO59" s="92"/>
       <c r="BV59" s="11"/>
-      <c r="BW59" s="90"/>
-      <c r="BX59" s="90"/>
-      <c r="BY59" s="90"/>
-      <c r="BZ59" s="95"/>
-      <c r="CA59" s="90"/>
-      <c r="CB59" s="90"/>
-      <c r="CC59" s="93"/>
-      <c r="CD59" s="90"/>
-      <c r="CE59" s="90"/>
-      <c r="CF59" s="90"/>
-      <c r="CG59" s="90"/>
-      <c r="CH59" s="90"/>
+      <c r="BW59" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="BX59" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY59" s="71"/>
+      <c r="BZ59" s="71"/>
+      <c r="CA59" s="75">
+        <v>45912</v>
+      </c>
+      <c r="CB59" s="71"/>
+      <c r="CC59" s="72"/>
+      <c r="CD59" s="76">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="CE59" s="71"/>
+      <c r="CF59" s="72"/>
+      <c r="CG59" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH59" s="78"/>
+      <c r="CI59" s="79"/>
+      <c r="CJ59" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="CP59" s="11" t="s">
         <v>9</v>
       </c>
@@ -29709,36 +29783,50 @@
         <v>126</v>
       </c>
       <c r="BF60" s="11"/>
-      <c r="BG60" s="95"/>
-      <c r="BH60" s="90"/>
-      <c r="BI60" s="90"/>
+      <c r="BG60" s="96"/>
+      <c r="BH60" s="92"/>
+      <c r="BI60" s="92"/>
       <c r="BJ60" s="93"/>
-      <c r="BK60" s="90"/>
-      <c r="BL60" s="90"/>
-      <c r="BM60" s="90"/>
-      <c r="BN60" s="90"/>
-      <c r="BO60" s="90"/>
+      <c r="BK60" s="92"/>
+      <c r="BL60" s="92"/>
+      <c r="BM60" s="92"/>
+      <c r="BN60" s="92"/>
+      <c r="BO60" s="92"/>
       <c r="BV60" s="11"/>
-      <c r="BW60" s="90"/>
-      <c r="BX60" s="90"/>
-      <c r="BY60" s="90"/>
-      <c r="BZ60" s="95"/>
-      <c r="CA60" s="90"/>
-      <c r="CB60" s="90"/>
-      <c r="CC60" s="93"/>
-      <c r="CD60" s="90"/>
-      <c r="CE60" s="90"/>
-      <c r="CF60" s="90"/>
-      <c r="CG60" s="90"/>
-      <c r="CH60" s="90"/>
+      <c r="BW60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BX60" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="BY60" s="52"/>
+      <c r="BZ60" s="52"/>
+      <c r="CA60" s="56">
+        <v>45914</v>
+      </c>
+      <c r="CB60" s="52"/>
+      <c r="CC60" s="42"/>
+      <c r="CD60" s="51">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="CE60" s="52"/>
+      <c r="CF60" s="42"/>
+      <c r="CG60" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH60" s="65"/>
+      <c r="CI60" s="74"/>
+      <c r="CJ60" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="CP60" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="CQ60" s="96" t="s">
+      <c r="CQ60" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="CR60" s="96"/>
-      <c r="CS60" s="96"/>
+      <c r="CR60" s="95"/>
+      <c r="CS60" s="95"/>
       <c r="CT60" s="71" t="s">
         <v>22</v>
       </c>
@@ -29824,28 +29912,42 @@
         <v>13</v>
       </c>
       <c r="BF61" s="11"/>
-      <c r="BG61" s="92"/>
-      <c r="BH61" s="90"/>
-      <c r="BI61" s="90"/>
+      <c r="BG61" s="91"/>
+      <c r="BH61" s="92"/>
+      <c r="BI61" s="92"/>
       <c r="BJ61" s="93"/>
-      <c r="BK61" s="90"/>
-      <c r="BL61" s="90"/>
-      <c r="BM61" s="90"/>
-      <c r="BN61" s="90"/>
-      <c r="BO61" s="90"/>
+      <c r="BK61" s="92"/>
+      <c r="BL61" s="92"/>
+      <c r="BM61" s="92"/>
+      <c r="BN61" s="92"/>
+      <c r="BO61" s="92"/>
       <c r="BV61" s="11"/>
-      <c r="BW61" s="90"/>
-      <c r="BX61" s="90"/>
-      <c r="BY61" s="90"/>
-      <c r="BZ61" s="92"/>
-      <c r="CA61" s="90"/>
-      <c r="CB61" s="90"/>
-      <c r="CC61" s="93"/>
-      <c r="CD61" s="90"/>
-      <c r="CE61" s="90"/>
-      <c r="CF61" s="90"/>
-      <c r="CG61" s="90"/>
-      <c r="CH61" s="90"/>
+      <c r="BW61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="BX61" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="BY61" s="52"/>
+      <c r="BZ61" s="52"/>
+      <c r="CA61" s="59">
+        <v>45914</v>
+      </c>
+      <c r="CB61" s="52"/>
+      <c r="CC61" s="42"/>
+      <c r="CD61" s="64">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="CE61" s="65"/>
+      <c r="CF61" s="66"/>
+      <c r="CG61" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH61" s="61"/>
+      <c r="CI61" s="62"/>
+      <c r="CJ61" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="CP61" s="11" t="s">
         <v>12</v>
       </c>
@@ -29939,28 +30041,39 @@
         <v>16</v>
       </c>
       <c r="BF62" s="11"/>
-      <c r="BG62" s="92"/>
-      <c r="BH62" s="90"/>
-      <c r="BI62" s="90"/>
+      <c r="BG62" s="91"/>
+      <c r="BH62" s="92"/>
+      <c r="BI62" s="92"/>
       <c r="BJ62" s="93"/>
-      <c r="BK62" s="90"/>
-      <c r="BL62" s="90"/>
-      <c r="BM62" s="90"/>
-      <c r="BN62" s="90"/>
-      <c r="BO62" s="90"/>
+      <c r="BK62" s="92"/>
+      <c r="BL62" s="92"/>
+      <c r="BM62" s="92"/>
+      <c r="BN62" s="92"/>
+      <c r="BO62" s="92"/>
       <c r="BV62" s="11"/>
-      <c r="BW62" s="90"/>
-      <c r="BX62" s="90"/>
-      <c r="BY62" s="90"/>
-      <c r="BZ62" s="92"/>
-      <c r="CA62" s="90"/>
-      <c r="CB62" s="90"/>
-      <c r="CC62" s="93"/>
-      <c r="CD62" s="90"/>
-      <c r="CE62" s="90"/>
-      <c r="CF62" s="90"/>
-      <c r="CG62" s="90"/>
-      <c r="CH62" s="90"/>
+      <c r="BW62" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX62" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY62" s="52"/>
+      <c r="BZ62" s="52"/>
+      <c r="CA62" s="68">
+        <v>45914</v>
+      </c>
+      <c r="CB62" s="65"/>
+      <c r="CC62" s="66"/>
+      <c r="CD62" s="51">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="CE62" s="52"/>
+      <c r="CF62" s="42"/>
+      <c r="CG62" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH62" s="61"/>
+      <c r="CI62" s="62"/>
       <c r="CP62" s="11" t="s">
         <v>14</v>
       </c>
@@ -30001,28 +30114,39 @@
     </row>
     <row r="63" spans="1:133 16340:16342">
       <c r="BF63" s="11"/>
-      <c r="BG63" s="92"/>
-      <c r="BH63" s="90"/>
-      <c r="BI63" s="90"/>
+      <c r="BG63" s="91"/>
+      <c r="BH63" s="92"/>
+      <c r="BI63" s="92"/>
       <c r="BJ63" s="93"/>
-      <c r="BK63" s="90"/>
-      <c r="BL63" s="90"/>
-      <c r="BM63" s="90"/>
-      <c r="BN63" s="90"/>
-      <c r="BO63" s="90"/>
+      <c r="BK63" s="92"/>
+      <c r="BL63" s="92"/>
+      <c r="BM63" s="92"/>
+      <c r="BN63" s="92"/>
+      <c r="BO63" s="92"/>
       <c r="BV63" s="11"/>
-      <c r="BW63" s="90"/>
-      <c r="BX63" s="90"/>
-      <c r="BY63" s="90"/>
-      <c r="BZ63" s="92"/>
-      <c r="CA63" s="90"/>
-      <c r="CB63" s="90"/>
-      <c r="CC63" s="93"/>
-      <c r="CD63" s="90"/>
-      <c r="CE63" s="90"/>
-      <c r="CF63" s="90"/>
-      <c r="CG63" s="90"/>
-      <c r="CH63" s="90"/>
+      <c r="BW63" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="BX63" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="BY63" s="63"/>
+      <c r="BZ63" s="63"/>
+      <c r="CA63" s="59">
+        <v>45914</v>
+      </c>
+      <c r="CB63" s="52"/>
+      <c r="CC63" s="42"/>
+      <c r="CD63" s="51">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="CE63" s="52"/>
+      <c r="CF63" s="42"/>
+      <c r="CG63" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH63" s="61"/>
+      <c r="CI63" s="62"/>
       <c r="CP63" s="11" t="s">
         <v>130</v>
       </c>
@@ -30036,7 +30160,7 @@
       </c>
       <c r="CU63" s="52"/>
       <c r="CV63" s="52"/>
-      <c r="CW63" s="91">
+      <c r="CW63" s="90">
         <v>45914</v>
       </c>
       <c r="CX63" s="65"/>
@@ -31139,7 +31263,12 @@
     <mergeCell ref="CW65:CY65"/>
     <mergeCell ref="CZ65:DB65"/>
     <mergeCell ref="DC65:DE65"/>
-    <mergeCell ref="CF63:CH63"/>
+    <mergeCell ref="CW62:CY62"/>
+    <mergeCell ref="CZ62:DB62"/>
+    <mergeCell ref="DC62:DE62"/>
+    <mergeCell ref="BG62:BI62"/>
+    <mergeCell ref="BJ62:BL62"/>
+    <mergeCell ref="BM62:BO62"/>
     <mergeCell ref="CQ63:CS63"/>
     <mergeCell ref="CT63:CV63"/>
     <mergeCell ref="CW63:CY63"/>
@@ -31148,39 +31277,28 @@
     <mergeCell ref="BG63:BI63"/>
     <mergeCell ref="BJ63:BL63"/>
     <mergeCell ref="BM63:BO63"/>
-    <mergeCell ref="BW63:BY63"/>
-    <mergeCell ref="BZ63:CB63"/>
-    <mergeCell ref="CC63:CE63"/>
-    <mergeCell ref="CF62:CH62"/>
-    <mergeCell ref="CQ62:CS62"/>
-    <mergeCell ref="CT62:CV62"/>
-    <mergeCell ref="CW62:CY62"/>
-    <mergeCell ref="CZ62:DB62"/>
-    <mergeCell ref="DC62:DE62"/>
-    <mergeCell ref="BG62:BI62"/>
-    <mergeCell ref="BJ62:BL62"/>
-    <mergeCell ref="BM62:BO62"/>
-    <mergeCell ref="BW62:BY62"/>
-    <mergeCell ref="BZ62:CB62"/>
-    <mergeCell ref="CC62:CE62"/>
+    <mergeCell ref="BX63:BZ63"/>
+    <mergeCell ref="CA63:CC63"/>
+    <mergeCell ref="CD63:CF63"/>
+    <mergeCell ref="CG63:CI63"/>
+    <mergeCell ref="BM61:BO61"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="U62:W62"/>
     <mergeCell ref="X62:Z62"/>
     <mergeCell ref="AN62:AP62"/>
     <mergeCell ref="AQ62:AS62"/>
-    <mergeCell ref="CF61:CH61"/>
     <mergeCell ref="CQ61:CS61"/>
     <mergeCell ref="CT61:CV61"/>
-    <mergeCell ref="CW61:CY61"/>
-    <mergeCell ref="CZ61:DB61"/>
-    <mergeCell ref="DC61:DE61"/>
-    <mergeCell ref="BG61:BI61"/>
-    <mergeCell ref="BJ61:BL61"/>
-    <mergeCell ref="BM61:BO61"/>
-    <mergeCell ref="BW61:BY61"/>
-    <mergeCell ref="BZ61:CB61"/>
-    <mergeCell ref="CC61:CE61"/>
+    <mergeCell ref="BX62:BZ62"/>
+    <mergeCell ref="CA62:CC62"/>
+    <mergeCell ref="CD62:CF62"/>
+    <mergeCell ref="CG62:CI62"/>
+    <mergeCell ref="CQ62:CS62"/>
+    <mergeCell ref="CT62:CV62"/>
+    <mergeCell ref="CA60:CC60"/>
+    <mergeCell ref="CD60:CF60"/>
+    <mergeCell ref="CG60:CI60"/>
     <mergeCell ref="CT60:CV60"/>
     <mergeCell ref="CW60:CY60"/>
     <mergeCell ref="CZ60:DB60"/>
@@ -31192,13 +31310,16 @@
     <mergeCell ref="AN61:AP61"/>
     <mergeCell ref="AQ61:AS61"/>
     <mergeCell ref="BM60:BO60"/>
-    <mergeCell ref="BW60:BY60"/>
-    <mergeCell ref="BZ60:CB60"/>
-    <mergeCell ref="CC60:CE60"/>
-    <mergeCell ref="CF60:CH60"/>
     <mergeCell ref="CQ60:CS60"/>
-    <mergeCell ref="CC59:CE59"/>
-    <mergeCell ref="CF59:CH59"/>
+    <mergeCell ref="BX61:BZ61"/>
+    <mergeCell ref="CA61:CC61"/>
+    <mergeCell ref="CD61:CF61"/>
+    <mergeCell ref="CG61:CI61"/>
+    <mergeCell ref="CW61:CY61"/>
+    <mergeCell ref="CZ61:DB61"/>
+    <mergeCell ref="DC61:DE61"/>
+    <mergeCell ref="BG61:BI61"/>
+    <mergeCell ref="BJ61:BL61"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="U60:W60"/>
@@ -31207,37 +31328,30 @@
     <mergeCell ref="AQ60:AS60"/>
     <mergeCell ref="BG60:BI60"/>
     <mergeCell ref="BJ60:BL60"/>
-    <mergeCell ref="CT48:CV48"/>
-    <mergeCell ref="CW48:CY48"/>
-    <mergeCell ref="CZ48:DB48"/>
-    <mergeCell ref="DC48:DE48"/>
+    <mergeCell ref="BX60:BZ60"/>
     <mergeCell ref="CW49:DE49"/>
     <mergeCell ref="BG59:BI59"/>
     <mergeCell ref="BJ59:BL59"/>
     <mergeCell ref="BM59:BO59"/>
-    <mergeCell ref="BW59:BY59"/>
-    <mergeCell ref="BZ59:CB59"/>
     <mergeCell ref="BG48:BI48"/>
     <mergeCell ref="BJ48:BL48"/>
     <mergeCell ref="BM48:BO48"/>
-    <mergeCell ref="BW48:BY48"/>
-    <mergeCell ref="BZ48:CH48"/>
     <mergeCell ref="CQ48:CS48"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="U48:W48"/>
-    <mergeCell ref="X48:Z48"/>
-    <mergeCell ref="AN48:AP48"/>
-    <mergeCell ref="AQ48:AS48"/>
-    <mergeCell ref="BG46:BO46"/>
+    <mergeCell ref="BX59:BZ59"/>
+    <mergeCell ref="CA59:CC59"/>
+    <mergeCell ref="CD59:CF59"/>
+    <mergeCell ref="CG59:CI59"/>
     <mergeCell ref="CQ46:CS46"/>
     <mergeCell ref="CW46:DE46"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="U47:Z47"/>
     <mergeCell ref="AN47:AP47"/>
     <mergeCell ref="BG47:BO47"/>
-    <mergeCell ref="BZ47:CH47"/>
     <mergeCell ref="CW47:DE47"/>
+    <mergeCell ref="CT48:CV48"/>
+    <mergeCell ref="CW48:CY48"/>
+    <mergeCell ref="CZ48:DB48"/>
+    <mergeCell ref="DC48:DE48"/>
     <mergeCell ref="DK18:DM18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="U19:W19"/>
@@ -31267,6 +31381,16 @@
     <mergeCell ref="AN9:AP9"/>
     <mergeCell ref="BG9:BI9"/>
     <mergeCell ref="BZ9:CB9"/>
+    <mergeCell ref="CA47:CI47"/>
+    <mergeCell ref="BX48:BZ48"/>
+    <mergeCell ref="CA48:CI48"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="U48:W48"/>
+    <mergeCell ref="X48:Z48"/>
+    <mergeCell ref="AN48:AP48"/>
+    <mergeCell ref="AQ48:AS48"/>
+    <mergeCell ref="BG46:BO46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>